<commit_message>
add webpage folder w express
</commit_message>
<xml_diff>
--- a/api-logging/Logs.xlsx
+++ b/api-logging/Logs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77b2c315ca72545e/Documents/Cat-Localizer/api-testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/77b2c315ca72545e/Documents/Cat-Localizer/api-logging/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="8_{21BC4CF8-399F-47C9-B797-6267D11B25ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F792A2F9-0474-480E-A60A-2E25E2C52DA2}"/>
+  <xr:revisionPtr revIDLastSave="96" documentId="8_{21BC4CF8-399F-47C9-B797-6267D11B25ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{965848AF-DFCB-4CAD-BE99-8E50A96588E3}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="16874" windowHeight="10574" xr2:uid="{8F297C9D-0AEF-44D3-A246-A891647753DF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{8F297C9D-0AEF-44D3-A246-A891647753DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="10">
   <si>
     <t>BLE_1</t>
   </si>
@@ -51,20 +51,26 @@
     <t>Location</t>
   </si>
   <si>
-    <t>living_room</t>
-  </si>
-  <si>
     <t>kitchen</t>
   </si>
   <si>
     <t>dining_room_1</t>
+  </si>
+  <si>
+    <t>dining_room_2</t>
+  </si>
+  <si>
+    <t>living_room_2</t>
+  </si>
+  <si>
+    <t>living_room_1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +114,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -129,7 +141,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -146,6 +158,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,10 +477,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FF66BA-5A84-4040-B44D-99964D2F6240}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:O156"/>
+  <dimension ref="A1:O261"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A42" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
+      <selection activeCell="I60" sqref="I60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.25" x14ac:dyDescent="0.7"/>
@@ -510,7 +525,7 @@
         <v>-66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F2" s="4"/>
       <c r="K2" s="4"/>
@@ -529,7 +544,7 @@
         <v>-110</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
@@ -555,7 +570,7 @@
         <v>-67</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
@@ -577,7 +592,7 @@
         <v>-70</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
@@ -599,7 +614,7 @@
         <v>-69</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K6" s="4"/>
       <c r="L6" s="4"/>
@@ -621,7 +636,7 @@
         <v>-67</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -643,7 +658,7 @@
         <v>-110</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -665,7 +680,7 @@
         <v>-74</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K9" s="4"/>
       <c r="L9" s="4"/>
@@ -687,7 +702,7 @@
         <v>-76</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
@@ -709,7 +724,7 @@
         <v>-76</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="4"/>
@@ -731,7 +746,7 @@
         <v>-75</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K12" s="4"/>
       <c r="L12" s="4"/>
@@ -753,7 +768,7 @@
         <v>-71</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
@@ -775,7 +790,7 @@
         <v>-73</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="4"/>
@@ -797,7 +812,7 @@
         <v>-110</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
@@ -819,7 +834,7 @@
         <v>-71</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K16" s="4"/>
       <c r="L16" s="4"/>
@@ -841,7 +856,7 @@
         <v>-89</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K17" s="4"/>
       <c r="L17" s="4"/>
@@ -863,7 +878,7 @@
         <v>-72</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K18" s="4"/>
       <c r="L18" s="4"/>
@@ -885,7 +900,7 @@
         <v>-80</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K19" s="4"/>
       <c r="L19" s="4"/>
@@ -907,7 +922,7 @@
         <v>-73</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K20" s="4"/>
       <c r="L20" s="4"/>
@@ -929,7 +944,7 @@
         <v>-73</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K21" s="4"/>
       <c r="L21" s="4"/>
@@ -951,7 +966,7 @@
         <v>-110</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
@@ -973,7 +988,7 @@
         <v>-80</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K23" s="4"/>
       <c r="L23" s="4"/>
@@ -995,7 +1010,7 @@
         <v>-110</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K24" s="4"/>
       <c r="L24" s="4"/>
@@ -1017,7 +1032,7 @@
         <v>-79</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4"/>
@@ -1039,7 +1054,7 @@
         <v>-86</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4"/>
@@ -1061,7 +1076,7 @@
         <v>-76</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4"/>
@@ -1083,7 +1098,7 @@
         <v>-88</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K28" s="4"/>
       <c r="L28" s="4"/>
@@ -1105,7 +1120,7 @@
         <v>-78</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -1127,7 +1142,7 @@
         <v>-82</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
@@ -1149,7 +1164,7 @@
         <v>-79</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K31" s="4"/>
       <c r="L31" s="4"/>
@@ -1171,7 +1186,7 @@
         <v>-81</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K32" s="4"/>
       <c r="L32" s="4"/>
@@ -1193,7 +1208,7 @@
         <v>-75</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K33" s="4"/>
       <c r="L33" s="4"/>
@@ -1215,7 +1230,7 @@
         <v>-78</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K34" s="4"/>
       <c r="L34" s="4"/>
@@ -1237,7 +1252,7 @@
         <v>-80</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
@@ -1259,7 +1274,7 @@
         <v>-76</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K36" s="4"/>
       <c r="L36" s="4"/>
@@ -1281,7 +1296,7 @@
         <v>-66</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K37" s="4"/>
       <c r="L37" s="4"/>
@@ -1303,7 +1318,7 @@
         <v>-69</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="K38" s="4"/>
       <c r="L38" s="4"/>
@@ -1325,7 +1340,7 @@
         <v>-67</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.7">
@@ -1342,7 +1357,7 @@
         <v>-68</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.7">
@@ -1359,7 +1374,7 @@
         <v>-110</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.7">
@@ -1376,7 +1391,7 @@
         <v>-68</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.7">
@@ -1393,7 +1408,7 @@
         <v>-66</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.7">
@@ -1410,7 +1425,7 @@
         <v>-65</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.7">
@@ -1427,7 +1442,7 @@
         <v>-65</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.7">
@@ -1444,7 +1459,7 @@
         <v>-67</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.7">
@@ -1461,7 +1476,7 @@
         <v>-68</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.7">
@@ -1478,7 +1493,7 @@
         <v>-75</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.7">
@@ -1495,7 +1510,7 @@
         <v>-75</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.7">
@@ -1512,7 +1527,7 @@
         <v>-75</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.7">
@@ -1529,7 +1544,7 @@
         <v>-77</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.7">
@@ -1546,7 +1561,7 @@
         <v>-68</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.7">
@@ -1563,7 +1578,7 @@
         <v>-72</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.7">
@@ -1580,7 +1595,7 @@
         <v>-88</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.7">
@@ -1597,7 +1612,7 @@
         <v>-82</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.7">
@@ -1614,7 +1629,7 @@
         <v>-110</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.7">
@@ -1631,7 +1646,7 @@
         <v>-86</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.7">
@@ -1648,7 +1663,7 @@
         <v>-74</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.7">
@@ -1665,7 +1680,7 @@
         <v>-76</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.7">
@@ -1682,7 +1697,7 @@
         <v>-72</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.7">
@@ -1699,7 +1714,7 @@
         <v>-76</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.7">
@@ -1716,7 +1731,7 @@
         <v>-79</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.7">
@@ -1733,7 +1748,7 @@
         <v>-87</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.7">
@@ -1750,7 +1765,7 @@
         <v>-80</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.7">
@@ -1767,7 +1782,7 @@
         <v>-82</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.7">
@@ -1784,7 +1799,7 @@
         <v>-87</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.7">
@@ -1801,7 +1816,7 @@
         <v>-110</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.7">
@@ -1818,7 +1833,7 @@
         <v>-110</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.7">
@@ -1835,7 +1850,7 @@
         <v>-75</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.7">
@@ -1852,7 +1867,7 @@
         <v>-77</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.7">
@@ -1869,7 +1884,7 @@
         <v>-75</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.7">
@@ -1886,7 +1901,7 @@
         <v>-78</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.7">
@@ -1903,7 +1918,7 @@
         <v>-110</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.7">
@@ -1920,7 +1935,7 @@
         <v>-74</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.7">
@@ -1937,7 +1952,7 @@
         <v>-110</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.7">
@@ -1954,7 +1969,7 @@
         <v>-68</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.7">
@@ -1971,7 +1986,7 @@
         <v>-71</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.7">
@@ -1988,7 +2003,7 @@
         <v>-80</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.7">
@@ -2005,7 +2020,7 @@
         <v>-110</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.7">
@@ -2022,7 +2037,7 @@
         <v>-80</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.7">
@@ -2039,7 +2054,7 @@
         <v>-78</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.7">
@@ -2056,7 +2071,7 @@
         <v>-110</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.7">
@@ -2073,7 +2088,7 @@
         <v>-73</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.7">
@@ -2090,7 +2105,7 @@
         <v>-110</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.7">
@@ -2107,7 +2122,7 @@
         <v>-68</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.7">
@@ -2124,7 +2139,7 @@
         <v>-73</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.7">
@@ -2141,7 +2156,7 @@
         <v>-74</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.7">
@@ -2158,7 +2173,7 @@
         <v>-63</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.7">
@@ -2175,7 +2190,7 @@
         <v>-63</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.7">
@@ -2192,7 +2207,7 @@
         <v>-63</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.7">
@@ -2209,7 +2224,7 @@
         <v>-110</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.7">
@@ -2226,7 +2241,7 @@
         <v>-74</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.7">
@@ -2243,7 +2258,7 @@
         <v>-110</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.7">
@@ -2260,7 +2275,7 @@
         <v>-69</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.7">
@@ -2277,7 +2292,7 @@
         <v>-69</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.7">
@@ -2294,7 +2309,7 @@
         <v>-70</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.7">
@@ -2311,7 +2326,7 @@
         <v>-60</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.7">
@@ -2328,7 +2343,7 @@
         <v>-69</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.7">
@@ -2345,7 +2360,7 @@
         <v>-68</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.7">
@@ -2362,7 +2377,7 @@
         <v>-67</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.7">
@@ -2379,7 +2394,7 @@
         <v>-65</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.7">
@@ -2396,7 +2411,7 @@
         <v>-110</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.7">
@@ -2413,7 +2428,7 @@
         <v>-110</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.7">
@@ -2430,7 +2445,7 @@
         <v>-69</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.7">
@@ -2447,7 +2462,7 @@
         <v>-71</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.7">
@@ -2464,7 +2479,7 @@
         <v>-110</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.7">
@@ -2481,7 +2496,7 @@
         <v>-62</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.7">
@@ -2498,7 +2513,7 @@
         <v>-64</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.7">
@@ -2515,7 +2530,7 @@
         <v>-63</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.7">
@@ -2532,7 +2547,7 @@
         <v>-59</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.7">
@@ -2549,7 +2564,7 @@
         <v>-62</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.7">
@@ -2566,7 +2581,7 @@
         <v>-60</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.7">
@@ -2583,7 +2598,7 @@
         <v>-67</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.7">
@@ -2600,7 +2615,7 @@
         <v>-110</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.7">
@@ -2617,7 +2632,7 @@
         <v>-66</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.7">
@@ -2634,7 +2649,7 @@
         <v>-110</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.7">
@@ -2651,7 +2666,7 @@
         <v>-72</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.7">
@@ -2668,7 +2683,7 @@
         <v>-110</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.7">
@@ -2685,7 +2700,7 @@
         <v>-71</v>
       </c>
       <c r="E119" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.7">
@@ -2702,7 +2717,7 @@
         <v>-110</v>
       </c>
       <c r="E120" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.7">
@@ -2719,7 +2734,7 @@
         <v>-71</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.7">
@@ -2736,7 +2751,7 @@
         <v>-56</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.7">
@@ -2753,7 +2768,7 @@
         <v>-57</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.7">
@@ -2770,7 +2785,7 @@
         <v>-56</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.7">
@@ -2787,7 +2802,7 @@
         <v>-59</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.7">
@@ -2804,7 +2819,7 @@
         <v>-57</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.7">
@@ -2821,7 +2836,7 @@
         <v>-61</v>
       </c>
       <c r="E127" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.7">
@@ -2838,7 +2853,7 @@
         <v>-36</v>
       </c>
       <c r="E128" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.7">
@@ -2855,7 +2870,7 @@
         <v>-35</v>
       </c>
       <c r="E129" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.7">
@@ -2872,7 +2887,7 @@
         <v>-38</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.7">
@@ -2889,7 +2904,7 @@
         <v>-35</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.7">
@@ -2906,7 +2921,7 @@
         <v>-50</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.7">
@@ -2923,7 +2938,7 @@
         <v>-57</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.7">
@@ -2940,7 +2955,7 @@
         <v>-57</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.7">
@@ -2957,7 +2972,7 @@
         <v>-57</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.7">
@@ -2974,7 +2989,7 @@
         <v>-57</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.7">
@@ -2991,7 +3006,7 @@
         <v>-56</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.7">
@@ -3008,7 +3023,7 @@
         <v>-53</v>
       </c>
       <c r="E138" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.7">
@@ -3025,7 +3040,7 @@
         <v>-56</v>
       </c>
       <c r="E139" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.7">
@@ -3042,7 +3057,7 @@
         <v>-55</v>
       </c>
       <c r="E140" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.7">
@@ -3059,7 +3074,7 @@
         <v>-53</v>
       </c>
       <c r="E141" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.7">
@@ -3076,7 +3091,7 @@
         <v>-57</v>
       </c>
       <c r="E142" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.7">
@@ -3093,7 +3108,7 @@
         <v>-53</v>
       </c>
       <c r="E143" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.7">
@@ -3110,7 +3125,7 @@
         <v>-55</v>
       </c>
       <c r="E144" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.7">
@@ -3127,7 +3142,7 @@
         <v>-55</v>
       </c>
       <c r="E145" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.7">
@@ -3144,7 +3159,7 @@
         <v>-55</v>
       </c>
       <c r="E146" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.7">
@@ -3161,7 +3176,7 @@
         <v>-57</v>
       </c>
       <c r="E147" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.7">
@@ -3178,7 +3193,7 @@
         <v>-46</v>
       </c>
       <c r="E148" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.7">
@@ -3195,7 +3210,7 @@
         <v>-49</v>
       </c>
       <c r="E149" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.7">
@@ -3212,7 +3227,7 @@
         <v>-45</v>
       </c>
       <c r="E150" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.7">
@@ -3229,7 +3244,7 @@
         <v>-46</v>
       </c>
       <c r="E151" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.7">
@@ -3246,7 +3261,7 @@
         <v>-49</v>
       </c>
       <c r="E152" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.7">
@@ -3263,7 +3278,7 @@
         <v>-56</v>
       </c>
       <c r="E153" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.7">
@@ -3280,7 +3295,7 @@
         <v>-54</v>
       </c>
       <c r="E154" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.7">
@@ -3297,7 +3312,7 @@
         <v>-55</v>
       </c>
       <c r="E155" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.7">
@@ -3314,7 +3329,1792 @@
         <v>-110</v>
       </c>
       <c r="E156" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A157" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B157" s="7">
+        <v>-45</v>
+      </c>
+      <c r="C157" s="7">
+        <v>-83</v>
+      </c>
+      <c r="D157" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E157" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A158" s="7">
+        <v>-86</v>
+      </c>
+      <c r="B158" s="7">
+        <v>-42</v>
+      </c>
+      <c r="C158" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D158" s="7">
+        <v>-77</v>
+      </c>
+      <c r="E158" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A159" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B159" s="7">
+        <v>-38</v>
+      </c>
+      <c r="C159" s="7">
+        <v>-71</v>
+      </c>
+      <c r="D159" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E159" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A160" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B160" s="7">
+        <v>-45</v>
+      </c>
+      <c r="C160" s="7">
+        <v>-80</v>
+      </c>
+      <c r="D160" s="7">
+        <v>-91</v>
+      </c>
+      <c r="E160" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A161" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B161" s="7">
+        <v>-37</v>
+      </c>
+      <c r="C161" s="7">
+        <v>-79</v>
+      </c>
+      <c r="D161" s="7">
+        <v>-91</v>
+      </c>
+      <c r="E161" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A162" s="7">
+        <v>-78</v>
+      </c>
+      <c r="B162" s="7">
+        <v>-37</v>
+      </c>
+      <c r="C162" s="7">
+        <v>-80</v>
+      </c>
+      <c r="D162" s="7">
+        <v>-87</v>
+      </c>
+      <c r="E162" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A163" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B163" s="7">
+        <v>-43</v>
+      </c>
+      <c r="C163" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D163" s="7">
+        <v>-77</v>
+      </c>
+      <c r="E163" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A164" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B164" s="7">
+        <v>-37</v>
+      </c>
+      <c r="C164" s="7">
+        <v>-77</v>
+      </c>
+      <c r="D164" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E164" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A165" s="7">
+        <v>-78</v>
+      </c>
+      <c r="B165" s="7">
+        <v>-45</v>
+      </c>
+      <c r="C165" s="7">
+        <v>-75</v>
+      </c>
+      <c r="D165" s="7">
+        <v>-77</v>
+      </c>
+      <c r="E165" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A166" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B166" s="7">
+        <v>-40</v>
+      </c>
+      <c r="C166" s="7">
+        <v>-71</v>
+      </c>
+      <c r="D166" s="7">
+        <v>-89</v>
+      </c>
+      <c r="E166" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A167" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B167" s="7">
+        <v>-50</v>
+      </c>
+      <c r="C167" s="7">
+        <v>-79</v>
+      </c>
+      <c r="D167" s="7">
+        <v>-80</v>
+      </c>
+      <c r="E167" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A168" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B168" s="7">
+        <v>-50</v>
+      </c>
+      <c r="C168" s="7">
+        <v>-72</v>
+      </c>
+      <c r="D168" s="7">
+        <v>-78</v>
+      </c>
+      <c r="E168" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A169" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B169" s="7">
+        <v>-49</v>
+      </c>
+      <c r="C169" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D169" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E169" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A170" s="7">
+        <v>-83</v>
+      </c>
+      <c r="B170" s="7">
+        <v>-48</v>
+      </c>
+      <c r="C170" s="7">
+        <v>-72</v>
+      </c>
+      <c r="D170" s="7">
+        <v>-79</v>
+      </c>
+      <c r="E170" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A171" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B171" s="7">
+        <v>-49</v>
+      </c>
+      <c r="C171" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D171" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E171" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A172" s="7">
+        <v>-84</v>
+      </c>
+      <c r="B172" s="7">
+        <v>-48</v>
+      </c>
+      <c r="C172" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D172" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E172" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A173" s="7">
+        <v>-80</v>
+      </c>
+      <c r="B173" s="7">
+        <v>-49</v>
+      </c>
+      <c r="C173" s="7">
+        <v>-72</v>
+      </c>
+      <c r="D173" s="7">
+        <v>-78</v>
+      </c>
+      <c r="E173" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A174" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B174" s="7">
+        <v>-48</v>
+      </c>
+      <c r="C174" s="7">
+        <v>-79</v>
+      </c>
+      <c r="D174" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E174" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A175" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B175" s="7">
+        <v>-49</v>
+      </c>
+      <c r="C175" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D175" s="7">
+        <v>-80</v>
+      </c>
+      <c r="E175" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A176" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B176" s="7">
+        <v>-50</v>
+      </c>
+      <c r="C176" s="7">
+        <v>-75</v>
+      </c>
+      <c r="D176" s="7">
+        <v>-79</v>
+      </c>
+      <c r="E176" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A177" s="7">
+        <v>-84</v>
+      </c>
+      <c r="B177" s="7">
+        <v>-47</v>
+      </c>
+      <c r="C177" s="7">
+        <v>-77</v>
+      </c>
+      <c r="D177" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E177" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A178" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B178" s="7">
+        <v>-55</v>
+      </c>
+      <c r="C178" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D178" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E178" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A179" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B179" s="7">
+        <v>-61</v>
+      </c>
+      <c r="C179" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D179" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E179" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A180" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B180" s="7">
+        <v>-55</v>
+      </c>
+      <c r="C180" s="7">
+        <v>-71</v>
+      </c>
+      <c r="D180" s="7">
+        <v>-79</v>
+      </c>
+      <c r="E180" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A181" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B181" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C181" s="7">
+        <v>-69</v>
+      </c>
+      <c r="D181" s="7">
+        <v>-78</v>
+      </c>
+      <c r="E181" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A182" s="7">
+        <v>-78</v>
+      </c>
+      <c r="B182" s="7">
+        <v>-61</v>
+      </c>
+      <c r="C182" s="7">
+        <v>-71</v>
+      </c>
+      <c r="D182" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E182" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="183" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A183" s="7">
+        <v>-83</v>
+      </c>
+      <c r="B183" s="7">
+        <v>-61</v>
+      </c>
+      <c r="C183" s="7">
+        <v>-68</v>
+      </c>
+      <c r="D183" s="7">
+        <v>-78</v>
+      </c>
+      <c r="E183" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="184" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A184" s="7">
+        <v>-86</v>
+      </c>
+      <c r="B184" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C184" s="7">
+        <v>-69</v>
+      </c>
+      <c r="D184" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E184" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="185" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A185" s="7">
+        <v>-89</v>
+      </c>
+      <c r="B185" s="7">
+        <v>-61</v>
+      </c>
+      <c r="C185" s="7">
+        <v>-70</v>
+      </c>
+      <c r="D185" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E185" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A186" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B186" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C186" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D186" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E186" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="187" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A187" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B187" s="7">
+        <v>-54</v>
+      </c>
+      <c r="C187" s="7">
+        <v>-71</v>
+      </c>
+      <c r="D187" s="7">
+        <v>-101</v>
+      </c>
+      <c r="E187" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A188" s="7">
+        <v>-84</v>
+      </c>
+      <c r="B188" s="7">
+        <v>-52</v>
+      </c>
+      <c r="C188" s="7">
+        <v>-73</v>
+      </c>
+      <c r="D188" s="7">
+        <v>-78</v>
+      </c>
+      <c r="E188" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A189" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B189" s="7">
+        <v>-53</v>
+      </c>
+      <c r="C189" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D189" s="7">
+        <v>-78</v>
+      </c>
+      <c r="E189" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="190" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A190" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B190" s="7">
+        <v>-51</v>
+      </c>
+      <c r="C190" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D190" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E190" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A191" s="7">
+        <v>-83</v>
+      </c>
+      <c r="B191" s="7">
+        <v>-52</v>
+      </c>
+      <c r="C191" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D191" s="7">
+        <v>-81</v>
+      </c>
+      <c r="E191" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A192" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B192" s="7">
+        <v>-51</v>
+      </c>
+      <c r="C192" s="7">
+        <v>-73</v>
+      </c>
+      <c r="D192" s="7">
+        <v>-79</v>
+      </c>
+      <c r="E192" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A193" s="7">
+        <v>-83</v>
+      </c>
+      <c r="B193" s="7">
+        <v>-50</v>
+      </c>
+      <c r="C193" s="7">
+        <v>-75</v>
+      </c>
+      <c r="D193" s="7">
+        <v>-82</v>
+      </c>
+      <c r="E193" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A194" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B194" s="7">
+        <v>-52</v>
+      </c>
+      <c r="C194" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D194" s="7">
+        <v>-81</v>
+      </c>
+      <c r="E194" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A195" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B195" s="7">
+        <v>-44</v>
+      </c>
+      <c r="C195" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D195" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E195" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A196" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B196" s="7">
+        <v>-55</v>
+      </c>
+      <c r="C196" s="7">
+        <v>-77</v>
+      </c>
+      <c r="D196" s="7">
+        <v>-88</v>
+      </c>
+      <c r="E196" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="197" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A197" s="7">
+        <v>-82</v>
+      </c>
+      <c r="B197" s="7">
+        <v>-49</v>
+      </c>
+      <c r="C197" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D197" s="7">
+        <v>-81</v>
+      </c>
+      <c r="E197" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A198" s="7">
+        <v>-83</v>
+      </c>
+      <c r="B198" s="7">
+        <v>-51</v>
+      </c>
+      <c r="C198" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D198" s="7">
+        <v>-81</v>
+      </c>
+      <c r="E198" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A199" s="7">
+        <v>-78</v>
+      </c>
+      <c r="B199" s="7">
+        <v>-47</v>
+      </c>
+      <c r="C199" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D199" s="7">
+        <v>-91</v>
+      </c>
+      <c r="E199" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="200" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A200" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B200" s="7">
+        <v>-44</v>
+      </c>
+      <c r="C200" s="7">
+        <v>-73</v>
+      </c>
+      <c r="D200" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E200" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A201" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B201" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C201" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D201" s="7">
+        <v>-87</v>
+      </c>
+      <c r="E201" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A202" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B202" s="7">
+        <v>-62</v>
+      </c>
+      <c r="C202" s="7">
+        <v>-78</v>
+      </c>
+      <c r="D202" s="7">
+        <v>-84</v>
+      </c>
+      <c r="E202" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A203" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B203" s="7">
+        <v>-50</v>
+      </c>
+      <c r="C203" s="7">
+        <v>-82</v>
+      </c>
+      <c r="D203" s="7">
+        <v>-84</v>
+      </c>
+      <c r="E203" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="204" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A204" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B204" s="7">
+        <v>-50</v>
+      </c>
+      <c r="C204" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D204" s="7">
+        <v>-83</v>
+      </c>
+      <c r="E204" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A205" s="7">
+        <v>-82</v>
+      </c>
+      <c r="B205" s="7">
+        <v>-51</v>
+      </c>
+      <c r="C205" s="7">
+        <v>-79</v>
+      </c>
+      <c r="D205" s="7">
+        <v>-90</v>
+      </c>
+      <c r="E205" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="206" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A206" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B206" s="7">
+        <v>-50</v>
+      </c>
+      <c r="C206" s="7">
+        <v>-86</v>
+      </c>
+      <c r="D206" s="7">
+        <v>-85</v>
+      </c>
+      <c r="E206" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A207" s="7">
+        <v>-80</v>
+      </c>
+      <c r="B207" s="7">
+        <v>-60</v>
+      </c>
+      <c r="C207" s="7">
+        <v>-74</v>
+      </c>
+      <c r="D207" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E207" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A208" s="7">
+        <v>-80</v>
+      </c>
+      <c r="B208" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C208" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D208" s="7">
+        <v>-84</v>
+      </c>
+      <c r="E208" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A209" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B209" s="7">
+        <v>-73</v>
+      </c>
+      <c r="C209" s="7">
+        <v>-70</v>
+      </c>
+      <c r="D209" s="7">
+        <v>-83</v>
+      </c>
+      <c r="E209" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A210" s="7">
+        <v>-79</v>
+      </c>
+      <c r="B210" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C210" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D210" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E210" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A211" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B211" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C211" s="7">
+        <v>-70</v>
+      </c>
+      <c r="D211" s="7">
+        <v>-83</v>
+      </c>
+      <c r="E211" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A212" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B212" s="7">
+        <v>-70</v>
+      </c>
+      <c r="C212" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D212" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E212" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A213" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B213" s="7">
+        <v>-56</v>
+      </c>
+      <c r="C213" s="7">
+        <v>-67</v>
+      </c>
+      <c r="D213" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E213" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A214" s="7">
+        <v>-80</v>
+      </c>
+      <c r="B214" s="7">
+        <v>-59</v>
+      </c>
+      <c r="C214" s="7">
+        <v>-63</v>
+      </c>
+      <c r="D214" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E214" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A215" s="7">
+        <v>-80</v>
+      </c>
+      <c r="B215" s="7">
+        <v>-58</v>
+      </c>
+      <c r="C215" s="7">
+        <v>-72</v>
+      </c>
+      <c r="D215" s="7">
+        <v>-84</v>
+      </c>
+      <c r="E215" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A216" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B216" s="7">
+        <v>-61</v>
+      </c>
+      <c r="C216" s="7">
+        <v>-60</v>
+      </c>
+      <c r="D216" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E216" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A217" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B217" s="7">
+        <v>-65</v>
+      </c>
+      <c r="C217" s="7">
+        <v>-62</v>
+      </c>
+      <c r="D217" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E217" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A218" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B218" s="7">
+        <v>-67</v>
+      </c>
+      <c r="C218" s="7">
+        <v>-61</v>
+      </c>
+      <c r="D218" s="7">
+        <v>-82</v>
+      </c>
+      <c r="E218" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A219" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B219" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C219" s="7">
+        <v>-67</v>
+      </c>
+      <c r="D219" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E219" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A220" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B220" s="7">
+        <v>-63</v>
+      </c>
+      <c r="C220" s="7">
+        <v>-61</v>
+      </c>
+      <c r="D220" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E220" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A221" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B221" s="7">
+        <v>-62</v>
+      </c>
+      <c r="C221" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D221" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E221" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A222" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B222" s="7">
+        <v>-72</v>
+      </c>
+      <c r="C222" s="7">
+        <v>-71</v>
+      </c>
+      <c r="D222" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E222" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A223" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B223" s="7">
+        <v>-72</v>
+      </c>
+      <c r="C223" s="7">
+        <v>-63</v>
+      </c>
+      <c r="D223" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E223" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A224" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B224" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C224" s="7">
+        <v>-68</v>
+      </c>
+      <c r="D224" s="7">
+        <v>-87</v>
+      </c>
+      <c r="E224" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A225" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B225" s="7">
+        <v>-67</v>
+      </c>
+      <c r="C225" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D225" s="7">
+        <v>-86</v>
+      </c>
+      <c r="E225" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A226" s="7">
+        <v>-84</v>
+      </c>
+      <c r="B226" s="7">
+        <v>-66</v>
+      </c>
+      <c r="C226" s="7">
+        <v>-55</v>
+      </c>
+      <c r="D226" s="7">
+        <v>-83</v>
+      </c>
+      <c r="E226" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A227" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B227" s="7">
+        <v>-63</v>
+      </c>
+      <c r="C227" s="7">
+        <v>-54</v>
+      </c>
+      <c r="D227" s="7">
+        <v>-84</v>
+      </c>
+      <c r="E227" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A228" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B228" s="7">
+        <v>-60</v>
+      </c>
+      <c r="C228" s="7">
+        <v>-52</v>
+      </c>
+      <c r="D228" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E228" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A229" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B229" s="7">
+        <v>-64</v>
+      </c>
+      <c r="C229" s="7">
+        <v>-52</v>
+      </c>
+      <c r="D229" s="7">
+        <v>-85</v>
+      </c>
+      <c r="E229" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A230" s="7">
+        <v>-86</v>
+      </c>
+      <c r="B230" s="7">
+        <v>-64</v>
+      </c>
+      <c r="C230" s="7">
+        <v>-54</v>
+      </c>
+      <c r="D230" s="7">
+        <v>-80</v>
+      </c>
+      <c r="E230" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A231" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B231" s="7">
+        <v>-66</v>
+      </c>
+      <c r="C231" s="7">
+        <v>-55</v>
+      </c>
+      <c r="D231" s="7">
+        <v>-83</v>
+      </c>
+      <c r="E231" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A232" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B232" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C232" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D232" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E232" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A233" s="7">
+        <v>-80</v>
+      </c>
+      <c r="B233" s="7">
+        <v>-67</v>
+      </c>
+      <c r="C233" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D233" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E233" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A234" s="7">
+        <v>-85</v>
+      </c>
+      <c r="B234" s="7">
+        <v>-67</v>
+      </c>
+      <c r="C234" s="7">
+        <v>-71</v>
+      </c>
+      <c r="D234" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E234" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A235" s="7">
+        <v>-81</v>
+      </c>
+      <c r="B235" s="7">
+        <v>-68</v>
+      </c>
+      <c r="C235" s="7">
+        <v>-70</v>
+      </c>
+      <c r="D235" s="7">
+        <v>-86</v>
+      </c>
+      <c r="E235" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A236" s="7">
+        <v>-86</v>
+      </c>
+      <c r="B236" s="7">
+        <v>-66</v>
+      </c>
+      <c r="C236" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D236" s="7">
+        <v>-81</v>
+      </c>
+      <c r="E236" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A237" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B237" s="7">
+        <v>-62</v>
+      </c>
+      <c r="C237" s="7">
+        <v>-73</v>
+      </c>
+      <c r="D237" s="7">
+        <v>-84</v>
+      </c>
+      <c r="E237" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A238" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B238" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C238" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D238" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E238" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A239" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B239" s="7">
+        <v>-65</v>
+      </c>
+      <c r="C239" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D239" s="7">
+        <v>-85</v>
+      </c>
+      <c r="E239" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A240" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B240" s="7">
+        <v>-62</v>
+      </c>
+      <c r="C240" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D240" s="7">
+        <v>-82</v>
+      </c>
+      <c r="E240" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A241" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B241" s="7">
+        <v>-62</v>
+      </c>
+      <c r="C241" s="7">
+        <v>-68</v>
+      </c>
+      <c r="D241" s="7">
+        <v>-84</v>
+      </c>
+      <c r="E241" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A242" s="7">
+        <v>-86</v>
+      </c>
+      <c r="B242" s="7">
+        <v>-63</v>
+      </c>
+      <c r="C242" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D242" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E242" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A243" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B243" s="7">
+        <v>-72</v>
+      </c>
+      <c r="C243" s="7">
+        <v>-78</v>
+      </c>
+      <c r="D243" s="7">
+        <v>-86</v>
+      </c>
+      <c r="E243" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A244" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B244" s="7">
+        <v>-71</v>
+      </c>
+      <c r="C244" s="7">
+        <v>-76</v>
+      </c>
+      <c r="D244" s="7">
+        <v>-87</v>
+      </c>
+      <c r="E244" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A245" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B245" s="7">
+        <v>-73</v>
+      </c>
+      <c r="C245" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D245" s="7">
+        <v>-88</v>
+      </c>
+      <c r="E245" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A246" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B246" s="7">
+        <v>-74</v>
+      </c>
+      <c r="C246" s="7">
+        <v>-79</v>
+      </c>
+      <c r="D246" s="7">
+        <v>-89</v>
+      </c>
+      <c r="E246" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A247" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B247" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C247" s="7">
+        <v>-78</v>
+      </c>
+      <c r="D247" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E247" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A248" s="7">
+        <v>-74</v>
+      </c>
+      <c r="B248" s="7">
+        <v>-63</v>
+      </c>
+      <c r="C248" s="7">
+        <v>-70</v>
+      </c>
+      <c r="D248" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E248" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A249" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B249" s="7">
+        <v>-110</v>
+      </c>
+      <c r="C249" s="7">
+        <v>-63</v>
+      </c>
+      <c r="D249" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E249" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A250" s="7">
+        <v>-78</v>
+      </c>
+      <c r="B250" s="7">
+        <v>-67</v>
+      </c>
+      <c r="C250" s="7">
+        <v>-68</v>
+      </c>
+      <c r="D250" s="7">
+        <v>-92</v>
+      </c>
+      <c r="E250" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A251" s="7">
+        <v>-77</v>
+      </c>
+      <c r="B251" s="7">
+        <v>-68</v>
+      </c>
+      <c r="C251" s="7">
+        <v>-60</v>
+      </c>
+      <c r="D251" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E251" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A252" s="7">
+        <v>-76</v>
+      </c>
+      <c r="B252" s="7">
+        <v>-64</v>
+      </c>
+      <c r="C252" s="7">
+        <v>-63</v>
+      </c>
+      <c r="D252" s="7">
+        <v>-80</v>
+      </c>
+      <c r="E252" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A253" s="7">
+        <v>-76</v>
+      </c>
+      <c r="B253" s="7">
+        <v>-62</v>
+      </c>
+      <c r="C253" s="7">
+        <v>-60</v>
+      </c>
+      <c r="D253" s="7">
+        <v>-93</v>
+      </c>
+      <c r="E253" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A254" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B254" s="7">
+        <v>-75</v>
+      </c>
+      <c r="C254" s="7">
+        <v>-64</v>
+      </c>
+      <c r="D254" s="7">
+        <v>-79</v>
+      </c>
+      <c r="E254" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A255" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B255" s="7">
+        <v>-76</v>
+      </c>
+      <c r="C255" s="7">
+        <v>-64</v>
+      </c>
+      <c r="D255" s="7">
+        <v>-86</v>
+      </c>
+      <c r="E255" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A256" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B256" s="7">
+        <v>-76</v>
+      </c>
+      <c r="C256" s="7">
+        <v>-62</v>
+      </c>
+      <c r="D256" s="7">
+        <v>-89</v>
+      </c>
+      <c r="E256" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A257" s="7">
+        <v>-75</v>
+      </c>
+      <c r="B257" s="7">
+        <v>-67</v>
+      </c>
+      <c r="C257" s="7">
+        <v>-62</v>
+      </c>
+      <c r="D257" s="7">
+        <v>-79</v>
+      </c>
+      <c r="E257" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A258" s="7">
+        <v>-75</v>
+      </c>
+      <c r="B258" s="7">
+        <v>-77</v>
+      </c>
+      <c r="C258" s="7">
+        <v>-60</v>
+      </c>
+      <c r="D258" s="7">
+        <v>-87</v>
+      </c>
+      <c r="E258" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A259" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B259" s="7">
+        <v>-73</v>
+      </c>
+      <c r="C259" s="7">
+        <v>-60</v>
+      </c>
+      <c r="D259" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E259" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A260" s="7">
+        <v>-76</v>
+      </c>
+      <c r="B260" s="7">
+        <v>-76</v>
+      </c>
+      <c r="C260" s="7">
+        <v>-110</v>
+      </c>
+      <c r="D260" s="7">
+        <v>-87</v>
+      </c>
+      <c r="E260" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.7">
+      <c r="A261" s="7">
+        <v>-110</v>
+      </c>
+      <c r="B261" s="7">
+        <v>-59</v>
+      </c>
+      <c r="C261" s="7">
+        <v>-63</v>
+      </c>
+      <c r="D261" s="7">
+        <v>-110</v>
+      </c>
+      <c r="E261" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>